<commit_message>
typo fix source spreadsheet
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/source/source_spreadsheets/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\capstat_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EEC9F67-43C1-406C-B9FA-0F9E0577FDE6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD59AF58-6F29-46C2-8E08-5ED795501A7C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="4" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
@@ -307,9 +307,6 @@
     <t>consumer-client</t>
   </si>
   <si>
-    <t>This profile defines the expected capabilities of a Da Vinci DEQM Consumer Client when conforming to the Da Vinci DEQM Implementation Guide.  Consumers include systems that are primary consumers of patient healthcare information and systems that consume data from Producers.   This CapabilityStatement resource includes the complete list of the *recommended*  Da Vinci DEQM profiles and RESTful operations that are  Da Vinci DEQM Consumer Client could support. Clients have the option of choosing from this list based on their local use cases and other contextual requirements.</t>
-  </si>
-  <si>
     <t>The DaVinci DEQM Consumer Client **SHOULD** be capable of supporting the DEQM MeasureReport Profiles and all the DEQM, CQFM and QI Core Profiles they reference.</t>
   </si>
   <si>
@@ -320,6 +317,9 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/cqfmeasures/ImplementationGuide/cqfmeasures</t>
+  </si>
+  <si>
+    <t>This profile defines the expected capabilities of a Da Vinci DEQM Consumer Client when conforming to the Da Vinci DEQM Implementation Guide.  Consumers include systems that are primary consumers of patient healthcare information and systems that consume data from Producers.   This CapabilityStatement resource includes the complete list of the *recommended*  Da Vinci DEQM profiles and RESTful operations that a Da Vinci DEQM Consumer Client could support. Clients have the option of choosing from this list based on their local use cases and other contextual requirements.</t>
   </si>
 </sst>
 </file>
@@ -753,7 +753,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -820,15 +820,15 @@
         <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1066,7 +1066,7 @@
         <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GF$21841 add note about coordination with Argonaut for subscription-based use cases and remove subscriptions
</commit_message>
<xml_diff>
--- a/source/source_spreadsheets/DEQM_Capability_Statement_Consumer_Client.xlsx
+++ b/source/source_spreadsheets/DEQM_Capability_Statement_Consumer_Client.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ERICS-AIR-2\ehaas\Documents\FHIR\Davinci-DEQM\source\source_spreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890ADA60-BDEE-4647-B82F-70830DE220D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B35D55D6-E141-4D79-B67C-955A96E6BFBB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="765" yWindow="555" windowWidth="28035" windowHeight="17445" activeTab="3" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
+    <workbookView xWindow="-28920" yWindow="-465" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{33C1B24A-521B-4A24-AA1F-999D8048322A}"/>
   </bookViews>
   <sheets>
     <sheet name="meta" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="94">
   <si>
     <t>Value</t>
   </si>
@@ -240,9 +240,6 @@
   </si>
   <si>
     <t>MedicationRequest</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/subscription-deqm</t>
   </si>
   <si>
     <t>Subscription</t>
@@ -320,6 +317,12 @@
   </si>
   <si>
     <t>The DaVinci DEQM Consumer Client **SHOULD** be capable of supporting the DEQM MeasureReport Profile and all the DEQM, CQFM and QI Core Profiles they reference.</t>
+  </si>
+  <si>
+    <t>!Subscription</t>
+  </si>
+  <si>
+    <t>!http://hl7.org/fhir/us/davinci-deqm/STU3/StructureDefinition/subscription-deqm</t>
   </si>
 </sst>
 </file>
@@ -745,7 +748,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="90" x14ac:dyDescent="0.25">
@@ -753,7 +756,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -769,7 +772,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -777,7 +780,7 @@
         <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -797,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0829A918-BBB6-6345-897C-371FBE4213DF}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,23 +815,23 @@
         <v>45</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -842,7 +845,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,7 +875,7 @@
         <v>51</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -886,7 +889,7 @@
         <v>53</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
@@ -900,7 +903,7 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -914,7 +917,7 @@
         <v>57</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
         <v>5</v>
@@ -928,7 +931,7 @@
         <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
@@ -942,7 +945,7 @@
         <v>61</v>
       </c>
       <c r="B7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
@@ -956,7 +959,7 @@
         <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
@@ -970,7 +973,7 @@
         <v>65</v>
       </c>
       <c r="B9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -981,16 +984,16 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1004,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACB4CFA-AAEF-4FC6-A49B-107CEE80A317}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,10 +1054,10 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1063,10 +1066,10 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -1109,16 +1112,16 @@
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>80</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1151,10 +1154,10 @@
         <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1162,7 +1165,7 @@
         <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1175,7 +1178,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1198,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>